<commit_message>
got contract created automatically to local server
</commit_message>
<xml_diff>
--- a/Amounts Mapping.xlsx
+++ b/Amounts Mapping.xlsx
@@ -1205,7 +1205,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1233,6 +1233,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF3CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1273,7 +1279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1335,6 +1341,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3034,36 +3047,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="80.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>157</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>196</v>
@@ -3072,68 +3085,68 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>11.13</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="14">
-        <v>11.13</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="26" t="s">
         <v>198</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="14">
-        <v>0.85</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="26" t="s">
         <v>200</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>2.61</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="14">
-        <v>2.61</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="26" t="s">
         <v>201</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="26" t="s">
         <v>202</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>13.74</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>186</v>
-      </c>
-      <c r="B8" s="14">
-        <v>13.74</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>203</v>
@@ -3142,12 +3155,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>1.05</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>187</v>
-      </c>
-      <c r="B9" s="14">
-        <v>1.05</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>205</v>
@@ -3156,12 +3169,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:5" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
+        <v>0</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>183</v>
-      </c>
-      <c r="B10" s="18">
-        <v>0</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>207</v>
@@ -3169,13 +3182,14 @@
       <c r="D10" s="20" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="1:5" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
+        <v>0</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>245</v>
-      </c>
-      <c r="B11" s="18">
-        <v>0</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>246</v>
@@ -3184,12 +3198,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>14.79</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>188</v>
-      </c>
-      <c r="B12" s="14">
-        <v>14.79</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>209</v>
@@ -3198,12 +3212,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>115</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="B13" s="14">
-        <v>115</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>211</v>
@@ -3212,12 +3226,12 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>2.06</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="B14" s="14">
-        <v>2.06</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>213</v>
@@ -3226,12 +3240,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>27</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="B15" s="14">
-        <v>27</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>214</v>
@@ -3240,12 +3254,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>8.77</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>179</v>
-      </c>
-      <c r="B16" s="14">
-        <v>8.77</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>216</v>
@@ -3255,11 +3269,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14">
+        <v>142</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>189</v>
-      </c>
-      <c r="B17" s="14">
-        <v>142</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>217</v>
@@ -3269,145 +3283,145 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="B19" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="B20" s="22" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="B21" s="22" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="B22" s="22" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="B23" s="21" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="B24" s="22" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="B26" s="21" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="B27" s="22" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="B28" s="21" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="B29" s="21" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="B30" s="22" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="B31" s="21" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+      <c r="B32" s="22" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+    <row r="33" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+    <row r="34" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
-    </row>
-    <row r="36" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+    <row r="35" spans="2:2" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="23"/>
+    </row>
+    <row r="36" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="24" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+    <row r="37" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="24" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+    <row r="38" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="24" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
+    <row r="39" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="24" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
+    <row r="40" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="24" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
+    <row r="41" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="24" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+    <row r="42" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="24" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
+    <row r="43" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="24" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
+    <row r="44" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="24" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
+    <row r="45" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="24" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
+    <row r="46" spans="2:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="24" t="s">
         <v>244</v>
       </c>
     </row>

</xml_diff>